<commit_message>
fixed p-value to correspond to an Ha of > in the Ethan Allen example
</commit_message>
<xml_diff>
--- a/docs/Data/DASL-HeliumFootball.xlsx
+++ b/docs/Data/DASL-HeliumFootball.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drp36\OneDrive - BYU-Idaho 1\221\Course_Files\BYUI_M221_Book\docs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drp36\OneDrive - BYU-Idaho 1\221\Course_Files\BYUI_M221_Book\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,7 +77,7 @@
     <t>controversy, "The Columbus Dispatch  (November, 21, 1993), B7.</t>
   </si>
   <si>
-    <t>that his leg would play no favorites if he tired or improved with practice</t>
+    <t>that his leg would play no favorites if he tired or improved with practice.</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>